<commit_message>
Changed simulation time to 4200s
</commit_message>
<xml_diff>
--- a/config/mdp_sumo_parameters.xlsx
+++ b/config/mdp_sumo_parameters.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KI4LSA\Code\github_repo\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KI4LSA\Code\LemgoRLTemp\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC71B31F-ED22-44F4-B560-3F79DC73DA2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E4A41C-3CA0-4882-9878-FC04F1186CB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -916,31 +916,31 @@
   <dimension ref="B1:AB27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="62.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="10" width="22.28515625" customWidth="1"/>
-    <col min="11" max="12" width="32.85546875" customWidth="1"/>
-    <col min="13" max="18" width="32.85546875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="30.28515625" style="4" customWidth="1"/>
-    <col min="20" max="22" width="30.28515625" style="3" customWidth="1"/>
-    <col min="23" max="25" width="28.5703125" customWidth="1"/>
-    <col min="26" max="28" width="28.5703125" style="3" customWidth="1"/>
-    <col min="29" max="30" width="28.5703125" customWidth="1"/>
-    <col min="31" max="1025" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="62.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
+    <col min="6" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="12" width="32.88671875" customWidth="1"/>
+    <col min="13" max="18" width="32.88671875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="30.33203125" style="4" customWidth="1"/>
+    <col min="20" max="22" width="30.33203125" style="3" customWidth="1"/>
+    <col min="23" max="25" width="28.5546875" customWidth="1"/>
+    <col min="26" max="28" width="28.5546875" style="3" customWidth="1"/>
+    <col min="29" max="30" width="28.5546875" customWidth="1"/>
+    <col min="31" max="1025" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
@@ -951,13 +951,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
@@ -965,10 +965,10 @@
         <v>35</v>
       </c>
       <c r="D3" s="12">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -979,7 +979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>49</v>
       </c>
@@ -990,7 +990,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>33</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>13.89</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>41</v>
       </c>
@@ -1078,11 +1078,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="5"/>
       <c r="D14" s="12"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>2</v>
       </c>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="D15" s="12"/>
     </row>
-    <row r="16" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>5</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="72" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>9</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>10</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>44</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>36</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>43</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>46</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>149.9</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Updated README and config
</commit_message>
<xml_diff>
--- a/config/mdp_sumo_parameters.xlsx
+++ b/config/mdp_sumo_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KI4LSA\Code\LemgoRLTemp\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KI4LSA\Code\LemgoRL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E4A41C-3CA0-4882-9878-FC04F1186CB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E468390-0C9D-4C67-8073-EB74ED1C7CF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>True</t>
   </si>
@@ -222,12 +222,6 @@
     <t>wait normalisation factor, s</t>
   </si>
   <si>
-    <t>wait_reward_coef</t>
-  </si>
-  <si>
-    <t>Balancing coefficient for wait in reward calculation</t>
-  </si>
-  <si>
     <t>Interaction period between agent and simulation.</t>
   </si>
   <si>
@@ -385,13 +379,49 @@
   </si>
   <si>
     <t>Distance from detector to junction, default=0.1m</t>
+  </si>
+  <si>
+    <t>wait_veh_reward_coef</t>
+  </si>
+  <si>
+    <t>wait_ped_reward_coef</t>
+  </si>
+  <si>
+    <r>
+      <t>α_veh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Balancing coefficient for wait_veh in reward calculation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>α_ped</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Balancing coefficient for wait_ped in reward calculation</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -459,6 +489,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -491,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -530,6 +566,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,13 +952,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AB27"/>
+  <dimension ref="B1:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,10 +998,10 @@
     </row>
     <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="12">
         <v>4200</v>
@@ -970,10 +1009,10 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="12">
         <v>2</v>
@@ -981,10 +1020,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="12">
         <v>90</v>
@@ -992,166 +1031,166 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>51</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="D7" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>52</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="12">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="12">
-        <v>14</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="12">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="12">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D12" s="12">
-        <v>13.89</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="12">
+        <v>13.89</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="12">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C14" s="5"/>
-      <c r="D14" s="12"/>
-    </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="12">
-        <v>120</v>
-      </c>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D18" s="12">
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+    <row r="19" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D19" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+    <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>0</v>
@@ -1159,67 +1198,78 @@
     </row>
     <row r="22" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D24" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
+    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="13">
+    </row>
+    <row r="26" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="13">
         <v>5.55</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
+    <row r="27" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="13">
+      <c r="D27" s="13">
         <v>149.9</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="11">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="11">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the mdp_sumo_parameters.xlsx to fix the key error
</commit_message>
<xml_diff>
--- a/config/mdp_sumo_parameters.xlsx
+++ b/config/mdp_sumo_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KI4LSA\Code\LemgoRL\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KI4LSA\Code\github_repo\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E468390-0C9D-4C67-8073-EB74ED1C7CF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CA8098-11FE-4A56-83AF-475747A97558}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>True</t>
   </si>
@@ -222,6 +222,12 @@
     <t>wait normalisation factor, s</t>
   </si>
   <si>
+    <t>wait_reward_coef</t>
+  </si>
+  <si>
+    <t>Balancing coefficient for wait in reward calculation</t>
+  </si>
+  <si>
     <t>Interaction period between agent and simulation.</t>
   </si>
   <si>
@@ -379,49 +385,13 @@
   </si>
   <si>
     <t>Distance from detector to junction, default=0.1m</t>
-  </si>
-  <si>
-    <t>wait_veh_reward_coef</t>
-  </si>
-  <si>
-    <t>wait_ped_reward_coef</t>
-  </si>
-  <si>
-    <r>
-      <t>α_veh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Balancing coefficient for wait_veh in reward calculation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>α_ped</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Balancing coefficient for wait_ped in reward calculation</t>
-    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -489,12 +459,6 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -527,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -566,9 +530,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,13 +913,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AB28"/>
+  <dimension ref="B1:AB27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -998,10 +959,10 @@
     </row>
     <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3" s="12">
         <v>4200</v>
@@ -1009,10 +970,10 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D4" s="12">
         <v>2</v>
@@ -1020,10 +981,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D5" s="12">
         <v>90</v>
@@ -1031,166 +992,166 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>53</v>
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="D7" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D8" s="12">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="12">
-        <v>0.2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" s="12">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="12">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D12" s="12">
-        <v>14</v>
+        <v>13.89</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D13" s="12">
-        <v>13.89</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="12">
-        <v>6</v>
-      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="5"/>
+      <c r="B15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="D15" s="12"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
-        <v>2</v>
+    <row r="16" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="12"/>
+        <v>19</v>
+      </c>
+      <c r="D16" s="12">
+        <v>120</v>
+      </c>
     </row>
     <row r="17" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="12">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="72" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D18" s="12">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>0</v>
@@ -1198,78 +1159,67 @@
     </row>
     <row r="22" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>36</v>
+      <c r="C25" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="13">
+        <v>5.55</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
-        <v>41</v>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D26" s="13">
-        <v>5.55</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>149.9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="13">
-        <v>149.9</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="11">
+        <v>52</v>
+      </c>
+      <c r="D27" s="11">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates in MDP relating to pedestrian processing and addition of pedestrian wait time evaluation.
</commit_message>
<xml_diff>
--- a/config/mdp_sumo_parameters.xlsx
+++ b/config/mdp_sumo_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KI4LSA\Code\github_repo\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KI4LSA\Code\LemgoRL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CA8098-11FE-4A56-83AF-475747A97558}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E468390-0C9D-4C67-8073-EB74ED1C7CF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>True</t>
   </si>
@@ -222,12 +222,6 @@
     <t>wait normalisation factor, s</t>
   </si>
   <si>
-    <t>wait_reward_coef</t>
-  </si>
-  <si>
-    <t>Balancing coefficient for wait in reward calculation</t>
-  </si>
-  <si>
     <t>Interaction period between agent and simulation.</t>
   </si>
   <si>
@@ -385,13 +379,49 @@
   </si>
   <si>
     <t>Distance from detector to junction, default=0.1m</t>
+  </si>
+  <si>
+    <t>wait_veh_reward_coef</t>
+  </si>
+  <si>
+    <t>wait_ped_reward_coef</t>
+  </si>
+  <si>
+    <r>
+      <t>α_veh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Balancing coefficient for wait_veh in reward calculation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>α_ped</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Balancing coefficient for wait_ped in reward calculation</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -459,6 +489,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -491,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -530,6 +566,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,13 +952,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AB27"/>
+  <dimension ref="B1:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,10 +998,10 @@
     </row>
     <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="12">
         <v>4200</v>
@@ -970,10 +1009,10 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="12">
         <v>2</v>
@@ -981,10 +1020,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="12">
         <v>90</v>
@@ -992,166 +1031,166 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>51</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="D7" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>52</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="12">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="12">
-        <v>14</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="12">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="12">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D12" s="12">
-        <v>13.89</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="12">
+        <v>13.89</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="12">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C14" s="5"/>
-      <c r="D14" s="12"/>
-    </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="12">
-        <v>120</v>
-      </c>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D18" s="12">
         <v>10000</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+    <row r="19" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D19" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+    <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>0</v>
@@ -1159,67 +1198,78 @@
     </row>
     <row r="22" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D24" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
+    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="13">
+    </row>
+    <row r="26" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="13">
         <v>5.55</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
+    <row r="27" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="13">
+      <c r="D27" s="13">
         <v>149.9</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="11">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="11">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated reward function and added normalizing factor for pedestrian.
</commit_message>
<xml_diff>
--- a/config/mdp_sumo_parameters.xlsx
+++ b/config/mdp_sumo_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KI4LSA\Code\LemgoRL\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\RL-Project\Code-Repo\ki4lsa\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E468390-0C9D-4C67-8073-EB74ED1C7CF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21F2244-858F-4DD7-BDA9-ABBE22E8358B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>True</t>
   </si>
@@ -415,6 +415,12 @@
       </rPr>
       <t xml:space="preserve"> Balancing coefficient for wait_ped in reward calculation</t>
     </r>
+  </si>
+  <si>
+    <t>ped_wait_norm</t>
+  </si>
+  <si>
+    <t>pedestrian wait normalisation factor</t>
   </si>
 </sst>
 </file>
@@ -572,7 +578,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -656,7 +662,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -952,16 +958,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AB28"/>
+  <dimension ref="B1:AB29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
@@ -1129,79 +1135,79 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="5"/>
-      <c r="D15" s="12"/>
+      <c r="B15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="12">
+        <v>100</v>
+      </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="12">
-        <v>120</v>
-      </c>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D19" s="12">
         <v>10000</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="s">
+    <row r="20" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D20" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
+    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>0</v>
@@ -1209,67 +1215,78 @@
     </row>
     <row r="23" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D25" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
+    <row r="26" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D26" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
+    <row r="27" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C27" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D27" s="13">
         <v>5.55</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D28" s="13">
         <v>149.9</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C29" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D29" s="11">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated pedestrian processing to improve wait time measurements based on speed and next edge of pedestrian. Also updated the ped_wait_norm value to 10.
</commit_message>
<xml_diff>
--- a/config/mdp_sumo_parameters.xlsx
+++ b/config/mdp_sumo_parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\RL-Project\Code-Repo\ki4lsa\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\RL-Project\Code-Repo\LemgoRL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21F2244-858F-4DD7-BDA9-ABBE22E8358B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEFF032-399F-43DD-BB2C-764A0CEAB711}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -964,7 +964,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,7 +1142,7 @@
         <v>56</v>
       </c>
       <c r="D15" s="12">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Algo config updates for rev 2.
</commit_message>
<xml_diff>
--- a/config/mdp_sumo_parameters.xlsx
+++ b/config/mdp_sumo_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\RL-Project\Code-Repo\LemgoRL\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\RL-Project\Code-Repo\ki4lsa\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEFF032-399F-43DD-BB2C-764A0CEAB711}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5890ED76-334D-4DFF-9657-D85FFED400CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>True</t>
   </si>
@@ -421,6 +421,12 @@
   </si>
   <si>
     <t>pedestrian wait normalisation factor</t>
+  </si>
+  <si>
+    <t>elapsed_norm</t>
+  </si>
+  <si>
+    <t>elapsed_time normalisation factor</t>
   </si>
 </sst>
 </file>
@@ -958,13 +964,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AB29"/>
+  <dimension ref="B1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,7 +1071,7 @@
         <v>54</v>
       </c>
       <c r="D8" s="12">
-        <v>1</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
@@ -1087,7 +1093,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="12">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
@@ -1098,7 +1104,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="12">
-        <v>45</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
@@ -1109,7 +1115,7 @@
         <v>26</v>
       </c>
       <c r="D12" s="12">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
@@ -1120,7 +1126,7 @@
         <v>38</v>
       </c>
       <c r="D13" s="12">
-        <v>13.89</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
@@ -1142,83 +1148,83 @@
         <v>56</v>
       </c>
       <c r="D15" s="12">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C16" s="5"/>
-      <c r="D16" s="12"/>
+      <c r="B16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="12">
+        <v>100</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="12">
-        <v>120</v>
-      </c>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D20" s="12">
         <v>10000</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
+    <row r="21" spans="2:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D21" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
+    <row r="22" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>0</v>
@@ -1226,67 +1232,78 @@
     </row>
     <row r="24" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D26" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
+    <row r="27" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D27" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
+    <row r="28" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D28" s="13">
         <v>5.55</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
+    <row r="29" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C29" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D29" s="13">
         <v>149.9</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C30" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D30" s="11">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>